<commit_message>
feat: fix bugs for grammar rules and add new templates
</commit_message>
<xml_diff>
--- a/resource/templates.xlsx
+++ b/resource/templates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\我的文档\张晗翀档案\大学\硕士\X-LANCE\text-to-SQL\项目\医疗数据库\medical-dataset\dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\我的文档\张晗翀档案\大学\硕士\X-LANCE\text-to-SQL\项目\医疗数据库\medical-dataset\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2560" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2752" uniqueCount="1340">
   <si>
     <t>一家医院调取患者之前在其他所有医院的就诊、检查数据，医保对可疑的就诊调取医院的就诊信息，与医保数据进行比对</t>
   </si>
@@ -4130,6 +4130,458 @@
   </si>
   <si>
     <t>SELECT OUT_DIAG_DIS_NM, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY OUT_DIAG_DIS_NM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某医院在某段时间内开出的检验报告单中，不同检测指标名称以及不同检测指标结果定量单位下，检测指标结果定量的平均值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医院（医疗机构代码）在（时间段）内开出的检验报告单中，不同检测指标名称以及不同检测指标结果定量单位下，检测指标结果定量的平均值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT JCZBMC, JCZBJGDW, AVG(JCZBJGDL) FROM jyjgzbb WHERE YLJGDM = $1 AND BGRQ BETWEEN $2 AND $3 GROUP BY JCZBMC, JCZBJGDW</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>科研人员</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某医院在某段时间内开出的检验报告单中，不同检测指标名称以及不同检测指标结果定量单位下，检测指标结果定量的平均值，并按平均值升序排序</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医院（医疗机构代码）在（时间段）内开出的检验报告单中，不同检测指标名称以及不同检测指标结果定量单位下，检测指标结果定量的平均值，并按平均值升序排序</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT JCZBMC, JCZBJGDW, AVG(JCZBJGDL) FROM jyjgzbb WHERE YLJGDM = $1 AND BGRQ BETWEEN $2 AND $3 GROUP BY JCZBMC, JCZBJGDW ORDER BY AVG(JCZBJGDL) ASC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某医院在某段时间内开出的检验报告单中，不同检测指标名称以及不同检测指标结果定量单位下，检测指标结果定量的平均值，并按平均值降序排序</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医院（医疗机构代码）在（时间段）内开出的检验报告单中，不同检测指标名称以及不同检测指标结果定量单位下，检测指标结果定量的平均值，并按平均值降序排序</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT JCZBMC, JCZBJGDW, AVG(JCZBJGDL) FROM jyjgzbb WHERE YLJGDM = $1 AND BGRQ BETWEEN $2 AND $3 GROUP BY JCZBMC, JCZBJGDW ORDER BY AVG(JCZBJGDL) DESC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医疗表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>科研人员</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某医院在某段时间内开出的检验报告单中，不同检测指标名称以及不同检测指标结果定量单位下，检测指标结果定量的平均值，保留平均值最小的若干项</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医院（医疗机构代码）在（时间段）内开出的检验报告单中，不同检测指标名称以及不同检测指标结果定量单位下，检测指标结果定量的平均值，保留平均值最小的（整数）项</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT JCZBMC, JCZBJGDW, AVG(JCZBJGDL) FROM jyjgzbb WHERE YLJGDM = $1 AND BGRQ BETWEEN $2 AND $3 GROUP BY JCZBMC, JCZBJGDW ORDER BY AVG(JCZBJGDL) ASC LIMIT $4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某医院在某段时间内开出的检验报告单中，不同检测指标名称以及不同检测指标结果定量单位下，检测指标结果定量的平均值，保留平均值最大的若干项</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医院（医疗机构代码）在（时间段）内开出的检验报告单中，不同检测指标名称以及不同检测指标结果定量单位下，检测指标结果定量的平均值，保留平均值最大的（整数）项</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT JCZBMC, JCZBJGDW, AVG(JCZBJGDL) FROM jyjgzbb WHERE YLJGDM = $1 AND BGRQ BETWEEN $2 AND $3 GROUP BY JCZBMC, JCZBJGDW ORDER BY AVG(JCZBJGDL) DESC LIMIT $4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内入院诊断疾病结果与出院诊断疾病结果不同的次数</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内入院诊断疾病结果与出院诊断疾病结果不同的次数</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内入院诊断疾病结果与出院诊断疾病结果不同的医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内入院诊断疾病结果与出院诊断疾病结果不同的医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT (SELECT COUNT(*) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3) - (SELECT COUNT(*) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND IN_DIAG_DIS_CD = OUT_DIAG_DIS_CD)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND IN_DIAG_DIS_CD &lt;&gt; OUT_DIAG_DIS_CD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3) EXCEPT (SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND IN_DIAG_DIS_CD = OUT_DIAG_DIS_CD)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某时间段内非某科室负责的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内非科室（科室编码）负责的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND MED_ORG_DEPT_CD &lt;&gt; $4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内非科室（科室名称）负责的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内非科室（科室名称）负责的所有医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3) EXCEPT (SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND MED_ORG_DEPT_CD = $4)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND MED_ORG_DEPT_NM &lt;&gt; $4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3) EXCEPT (SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND MED_ORG_DEPT_NM = $4)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出某医院在某时间段内所有非异地结算的医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>列出医院（医疗机构代码）在（时间段）内所有非异地结算的医疗就诊记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND REMOTE_SETTLE_FLG = 0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3) EXCEPT (SELECT * FROM t_kc21 WHERE MED_SER_ORG_NO = $1 AND IN_HOSP_DATE BETWEEN $2 AND $3 AND (REMOTE_SETTLE_FLG = 1 OR REMOTE_SETTLE_FLG = 2))</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室编码和入院诊断疾病编码，列出某医院所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室编码和入院诊断疾病编码，列出医院（医疗机构代码）所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_CD, IN_DIAG_DIS_CD, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD, IN_DIAG_DIS_CD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室编码和入院诊断疾病名称，列出某医院所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室编码和出院诊断疾病编码，列出某医院所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室编码和出院诊断疾病名称，列出某医院所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和入院诊断疾病编码，列出某医院所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和入院诊断疾病名称，列出某医院所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和出院诊断疾病编码，列出某医院所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和出院诊断疾病名称，列出某医院所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和入院诊断疾病编码，列出医院（医疗机构代码）所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室编码和出院诊断疾病编码，列出医院（医疗机构代码）所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和出院诊断疾病编码，列出医院（医疗机构代码）所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室编码和入院诊断疾病名称，列出医院（医疗机构代码）所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室编码和出院诊断疾病名称，列出医院（医疗机构代码）所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和入院诊断疾病名称，列出医院（医疗机构代码）所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和出院诊断疾病名称，列出医院（医疗机构代码）所有医疗就诊记录中患者的平均年龄</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_CD, IN_DIAG_DIS_NM, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD, IN_DIAG_DIS_NM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_CD, OUT_DIAG_DIS_CD, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD, OUT_DIAG_DIS_CD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_CD, OUT_DIAG_DIS_NM, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_CD, OUT_DIAG_DIS_NM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_NM, IN_DIAG_DIS_CD, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_NM, IN_DIAG_DIS_CD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_NM, IN_DIAG_DIS_NM, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_NM, IN_DIAG_DIS_NM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_NM, OUT_DIAG_DIS_CD, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_NM, OUT_DIAG_DIS_CD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_NM, OUT_DIAG_DIS_NM, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_NM, OUT_DIAG_DIS_NM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和入院诊断疾病名称，列出某医院所有医疗就诊记录中患者的平均年龄，保留平均年龄小于（整数）岁的记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和出院诊断疾病名称，列出某医院所有医疗就诊记录中患者的平均年龄，保留平均年龄大于（整数）岁的记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和入院诊断疾病名称，列出医院（医疗机构代码）所有医疗就诊记录中患者的平均年龄，保留平均年龄小于（整数）岁的记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的科室名称和出院诊断疾病名称，列出医院（医疗机构代码）所有医疗就诊记录中患者的平均年龄，保留平均年龄大于（整数）岁的记录</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_NM, IN_DIAG_DIS_NM, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_NM, IN_DIAG_DIS_NM HAVING AVG(PERSON_AGE) &lt; $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT MED_ORG_DEPT_NM, OUT_DIAG_DIS_NM, AVG(PERSON_AGE) FROM t_kc21 WHERE MED_SER_ORG_NO = $1 GROUP BY MED_ORG_DEPT_NM, OUT_DIAG_DIS_NM HAVING AVG(PERSON_AGE) &gt; $2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>某医院在某段时间内所有医疗记录的个人账户支出与医疗费总额的平均比值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医院（医疗机构代码）在（时间段）内所有医疗记录的个人账户支出与医疗费总额的平均比值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT AVG(t_kc24.PER_ACC_PAY / t_kc24.MED_AMOUT) FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 AND t_kc24.CLINIC_SLT_DATE BETWEEN $2 AND $3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同科室编码下，列出某医院所有医疗就诊记录的统筹基金支出与医疗费总额的平均比值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同科室编码下，列出医院（医疗机构代码）所有医疗就诊记录的统筹基金支出与医疗费总额的平均比值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT t_kc21.MED_ORG_DEPT_CD, AVG(t_kc24.OVE_PAY / t_kc24.MED_AMOUT) FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 GROUP BY t_kc21.MED_ORG_DEPT_CD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>复杂</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同科室名称下，列出某医院所有医疗就诊记录的统筹基金支出与医疗费总额的平均比值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同科室名称下，列出医院（医疗机构代码）所有医疗就诊记录的统筹基金支出与医疗费总额的平均比值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT t_kc21.MED_ORG_DEPT_NM, AVG(t_kc24.OVE_PAY / t_kc24.MED_AMOUT) FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 GROUP BY t_kc22.MED_ORG_DEPT_NM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同科室编码和入院诊断疾病编码下，列出某医院所有医疗就诊记录的大病支付与医疗费总额的比值的最小值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同科室编码和入院诊断疾病编码下，列出医院（医疗机构代码）所有医疗就诊记录的大病支付与医疗费总额的比值的最小值</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT t_kc21.MED_ORG_DEPT_CD, t_kc21.IN_DIAG_DIS_CD, MIN(t_kc24.ILL_PAY / t_kc24.MED_AMOUT) FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 GROUP BY t_kc21.MED_ORG_DEPT_CD, t_kc21.IN_DIAG_DIS_CD</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保表</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>医保</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同科室编码和入院诊断疾病名称下，列出某医院所有医疗就诊记录的民政补助与医疗费总额的比值的最大值，并降序排序</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同科室编码和入院诊断疾病名称下，列出医院（医疗机构代码）所有医疗就诊记录的民政补助与医疗费总额的比值的最大值，并降序排序</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT t_kc21.MED_ORG_DEPT_CD, t_kc21.IN_DIAG_DIS_NM, MAX(t_kc24.CIVIL_SUBSIDY / t_kc24.MED_AMOUT) FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 GROUP BY t_kc21.MED_ORG_DEPT_CD, t_kc21.IN_DIAG_DIS_NM ORDER BY MAX(t_kc24.CIVIL_SUBSIDY / t_kc24.MED_AMOUT) DESC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同科室名称和出院诊断疾病编码下，列出某医院所有医疗就诊记录的个人自费与医疗费总额的比值的最小值，并升序排序</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不同科室名称和出院诊断疾病编码下，列出医院（医疗机构代码）所有医疗就诊记录的个人自费与医疗费总额的比值的最小值，并升序排序</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT t_kc21.MED_ORG_DEPT_NM, t_kc21.OUT_DIAG_DIS_CD, MIN(t_kc24.PER_EXP / t_kc24.MED_AMOUT) FROM t_kc21 JOIN t_kc24 ON t_kc21.MED_CLINIC_ID = t_kc24.MED_CLINIC_ID WHERE t_kc21.MED_SER_ORG_NO = $1 GROUP BY t_kc21.MED_ORG_DEPT_NM, t_kc21.OUT_DIAG_DIS_CD ORDER BY MIN(t_kc24.PER_EXP / t_kc24.MED_AMOUT) ASC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算某条医疗费用明细记录中药品的数量与单价的乘积</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算医疗费用明细记录（人员医疗费用明细ID）中药品的数量与单价的乘积</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT QTY * UNIVALENT FROM t_kc22 WHERE MED_EXP_DET_ID = $1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>验证某条医疗费用明细记录中药品的数量与单价的乘积是否等于药品的金额</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>验证医疗费用明细记录（人员医疗费用明细ID）中药品的数量与单价的乘积是否等于药品的金额</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SELECT (SELECT QTY * UNIVALENT FROM t_kc22 WHERE MED_EXP_DET_ID = $1) = (SELECT AMOUNT FROM t_kc22 WHERE MED_EXP_DET_ID = $1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>患者</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4522,14 +4974,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB435"/>
+  <dimension ref="A1:AB467"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="103.21875" customWidth="1"/>
-    <col min="2" max="2" width="140.77734375" customWidth="1"/>
+    <col min="1" max="1" width="131.5546875" customWidth="1"/>
+    <col min="2" max="2" width="150.33203125" customWidth="1"/>
     <col min="3" max="3" width="255.77734375" customWidth="1"/>
     <col min="4" max="28" width="14" customWidth="1"/>
   </cols>
@@ -21410,6 +21862,742 @@
         <v>1217</v>
       </c>
     </row>
+    <row r="436" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A436" s="1" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B436" s="1" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C436" s="1" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D436" s="5" t="s">
+        <v>1230</v>
+      </c>
+      <c r="E436" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F436" s="5">
+        <v>3</v>
+      </c>
+      <c r="G436" s="5" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="437" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A437" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B437" s="1" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>1235</v>
+      </c>
+      <c r="D437" s="5" t="s">
+        <v>1230</v>
+      </c>
+      <c r="E437" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F437" s="5">
+        <v>3</v>
+      </c>
+      <c r="G437" s="5" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="438" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A438" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B438" s="1" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C438" s="1" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D438" s="5" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E438" s="5" t="s">
+        <v>1240</v>
+      </c>
+      <c r="F438" s="5">
+        <v>3</v>
+      </c>
+      <c r="G438" s="5" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="439" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A439" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B439" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D439" s="5" t="s">
+        <v>1230</v>
+      </c>
+      <c r="E439" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="F439" s="5">
+        <v>3</v>
+      </c>
+      <c r="G439" s="5" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="440" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A440" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B440" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D440" s="5" t="s">
+        <v>1239</v>
+      </c>
+      <c r="E440" s="5" t="s">
+        <v>1240</v>
+      </c>
+      <c r="F440" s="5">
+        <v>3</v>
+      </c>
+      <c r="G440" s="5" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="441" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A441" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B441" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C441" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D441" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E441" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F441" s="5">
+        <v>6</v>
+      </c>
+      <c r="G441" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="442" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A442" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B442" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C442" s="1" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D442" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E442" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F442" s="5">
+        <v>6</v>
+      </c>
+      <c r="G442" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="443" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A443" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B443" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C443" s="1" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D443" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E443" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F443" s="5">
+        <v>6</v>
+      </c>
+      <c r="G443" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="444" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A444" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B444" s="1" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C444" s="1" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D444" s="4" t="s">
+        <v>1258</v>
+      </c>
+      <c r="E444" s="4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F444" s="5">
+        <v>6</v>
+      </c>
+      <c r="G444" s="4" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="445" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A445" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B445" s="1" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C445" s="1" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D445" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E445" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F445" s="5">
+        <v>6</v>
+      </c>
+      <c r="G445" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="446" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A446" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B446" s="1" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C446" s="1" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D446" s="4" t="s">
+        <v>1258</v>
+      </c>
+      <c r="E446" s="4" t="s">
+        <v>1259</v>
+      </c>
+      <c r="F446" s="5">
+        <v>6</v>
+      </c>
+      <c r="G446" s="4" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="447" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A447" s="1" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B447" s="1" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C447" s="1" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D447" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E447" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F447" s="5">
+        <v>6</v>
+      </c>
+      <c r="G447" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="448" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A448" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B448" s="1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C448" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D448" s="4" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E448" s="4" t="s">
+        <v>1269</v>
+      </c>
+      <c r="F448" s="5">
+        <v>6</v>
+      </c>
+      <c r="G448" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="449" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A449" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B449" s="1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C449" s="1" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D449" s="4" t="s">
+        <v>1268</v>
+      </c>
+      <c r="E449" s="4" t="s">
+        <v>1269</v>
+      </c>
+      <c r="F449" s="5">
+        <v>6</v>
+      </c>
+      <c r="G449" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="450" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A450" s="1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B450" s="1" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C450" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="D450" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E450" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F450" s="5">
+        <v>6</v>
+      </c>
+      <c r="G450" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="451" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A451" s="1" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B451" s="1" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C451" s="1" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D451" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E451" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F451" s="5">
+        <v>6</v>
+      </c>
+      <c r="G451" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="452" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A452" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B452" s="1" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C452" s="1" t="s">
+        <v>1292</v>
+      </c>
+      <c r="D452" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E452" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F452" s="5">
+        <v>6</v>
+      </c>
+      <c r="G452" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="453" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A453" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B453" s="1" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C453" s="1" t="s">
+        <v>1293</v>
+      </c>
+      <c r="D453" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E453" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F453" s="5">
+        <v>6</v>
+      </c>
+      <c r="G453" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="454" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A454" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="B454" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C454" s="1" t="s">
+        <v>1294</v>
+      </c>
+      <c r="D454" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E454" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F454" s="5">
+        <v>6</v>
+      </c>
+      <c r="G454" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="455" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A455" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B455" s="1" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C455" s="1" t="s">
+        <v>1295</v>
+      </c>
+      <c r="D455" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E455" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F455" s="5">
+        <v>6</v>
+      </c>
+      <c r="G455" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="456" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A456" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B456" s="1" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C456" s="1" t="s">
+        <v>1296</v>
+      </c>
+      <c r="D456" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E456" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F456" s="5">
+        <v>6</v>
+      </c>
+      <c r="G456" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="457" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A457" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B457" s="1" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C457" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="D457" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E457" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F457" s="5">
+        <v>6</v>
+      </c>
+      <c r="G457" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="458" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A458" s="1" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B458" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C458" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D458" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E458" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F458" s="5">
+        <v>6</v>
+      </c>
+      <c r="G458" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="459" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A459" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B459" s="1" t="s">
+        <v>1301</v>
+      </c>
+      <c r="C459" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D459" s="4" t="s">
+        <v>1275</v>
+      </c>
+      <c r="E459" s="4" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F459" s="5">
+        <v>6</v>
+      </c>
+      <c r="G459" s="4" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="460" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A460" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B460" s="1" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C460" s="1" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D460" s="4" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E460" s="4" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F460" s="5">
+        <v>6</v>
+      </c>
+      <c r="G460" s="4" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="461" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A461" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B461" s="1" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C461" s="1" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D461" s="4" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E461" s="4" t="s">
+        <v>1314</v>
+      </c>
+      <c r="F461" s="5">
+        <v>6</v>
+      </c>
+      <c r="G461" s="4" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="462" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A462" s="1" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B462" s="1" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C462" s="1" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D462" s="4" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E462" s="4" t="s">
+        <v>1314</v>
+      </c>
+      <c r="F462" s="5">
+        <v>6</v>
+      </c>
+      <c r="G462" s="4" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="463" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A463" s="1" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B463" s="1" t="s">
+        <v>1320</v>
+      </c>
+      <c r="C463" s="1" t="s">
+        <v>1321</v>
+      </c>
+      <c r="D463" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E463" s="4" t="s">
+        <v>1323</v>
+      </c>
+      <c r="F463" s="5">
+        <v>6</v>
+      </c>
+      <c r="G463" s="4" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="464" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A464" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B464" s="1" t="s">
+        <v>1325</v>
+      </c>
+      <c r="C464" s="1" t="s">
+        <v>1326</v>
+      </c>
+      <c r="D464" s="4" t="s">
+        <v>1322</v>
+      </c>
+      <c r="E464" s="4" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F464" s="5">
+        <v>6</v>
+      </c>
+      <c r="G464" s="4" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="465" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A465" s="1" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B465" s="1" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D465" s="4" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E465" s="4" t="s">
+        <v>1308</v>
+      </c>
+      <c r="F465" s="5">
+        <v>6</v>
+      </c>
+      <c r="G465" s="4" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="466" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A466" s="1" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B466" s="1" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C466" s="1" t="s">
+        <v>1332</v>
+      </c>
+      <c r="D466" s="4" t="s">
+        <v>1307</v>
+      </c>
+      <c r="E466" s="4" t="s">
+        <v>1333</v>
+      </c>
+      <c r="F466" s="5">
+        <v>8</v>
+      </c>
+      <c r="G466" s="4" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="467" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A467" s="1" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B467" s="1" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C467" s="1" t="s">
+        <v>1337</v>
+      </c>
+      <c r="D467" s="4" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E467" s="4" t="s">
+        <v>1338</v>
+      </c>
+      <c r="F467" s="5">
+        <v>8</v>
+      </c>
+      <c r="G467" s="4" t="s">
+        <v>1339</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>